<commit_message>
upd: - linen types edit - check linen edit - tables edit
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/белье_по комплектам.xlsx
+++ b/app/download_dir/system_files/белье_по комплектам.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="688">
   <si>
     <t xml:space="preserve">Код ТНВЭД</t>
   </si>
@@ -264,6 +264,9 @@
     <t xml:space="preserve">Тип разрешительной документации</t>
   </si>
   <si>
+    <t xml:space="preserve">БОРТИК</t>
+  </si>
+  <si>
     <t xml:space="preserve">БЕЖЕВЫЙ</t>
   </si>
   <si>
@@ -282,381 +285,441 @@
     <t xml:space="preserve">Значение атрибута</t>
   </si>
   <si>
+    <t xml:space="preserve">ДОРОЖКА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЖЕВЫЙ МЕЛАНЖ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ДЕТСКИЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НЕ ОПРЕДЕЛЕНО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АВСТРАЛИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ИЗДЕЛИЕ ДЛЯ БАНИ И САУНЫ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЖЕВЫЙ/ЗЕЛЕНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЛЮБОЙ ВОЗРАСТ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АКФИЛ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АВСТРИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сертификат</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОВРИК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЖЕВЫЙ/СИНИЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЗ УКАЗАНИЯ ВОЗРАСТА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АЗЕРБАЙДЖАН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модель / артикул производителя(тип)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модель</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОМПЛЕКТ ПОСТЕЛЬНОГО БЕЛЬЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЛО-ЗЕЛЕНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БАЙКА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АЛАНДСКИЕ ОСТРОВА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОНВЕРТ ДЛЯ ПРИБОРОВ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЛО-КОРИЧНЕВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БАТИСТ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АЛБАНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модель / Артикул</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОСТЕР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БИОМАТИН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АЛЖИР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МЕШОК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЛЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЯЗЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АМЕРИКАНСКИЕ ВИРГИНСКИЕ ОСТРОВА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НАВОЛОЧКА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЛЫЙ/БЕЖЕВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ВЕЛЮР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АМЕРИКАНСКОЕ САМОА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НАМАТРАСНИК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ВУАЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АНГИЛЬЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НАПЕРНИК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЛЫЙ/СИНИЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ВАФЕЛЬНОЕ ПОЛОТНО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АНГОЛА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НАПЕРОН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БИРЮЗОВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГАБАРДИН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АНДОРРА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПЕЛЁНКА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БОРДОВО-РЫЖИЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГОБЕЛЕН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АНТАРКТИДА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОДОДЕЯЛЬНИК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БОРДОВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ДАМАСТ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АНТИГУА И БАРБУДА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номер Регламента/стандарта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТР ТС 007/2011 "О безопасности продукции, предназначенной для детей и подростков"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОДСТАКАННИК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БРОНЗОВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ДЖЕРСИ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АРГЕНТИНА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТР ТС 017/2011 "О безопасности продукции легкой промышленности"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОДСТИЛКА ПОД БЛЮДО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ВАНИЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЖАККАРД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АРМЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТР ТС 005/2011 "О безопасности упаковки"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ВИШНЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КУЛИРНАЯ ГЛАДЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АРУБА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Действие технических регламентов не распространяется</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ БАННОЕ/КУПАЛЬНОЕ ПОЛОТЕНЦЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГОЛУБОЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЛЬНЯНАЯ ТКАНЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АФГАНИСТАН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ГОСТЕВОЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГОРЧИЧНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МАКО-САТИН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БАГАМЫ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ ВОЛОС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГРАФИТОВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МАХРОВАЯ ТКАНЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БАНГЛАДЕШ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ ЛИЦА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЖЁЛТЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МИКРОВОЛОКНО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БАРБАДОС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ НОГ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЗЕЛЁНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МИКРОПОЛИЕСТР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БАХРЕЙН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ РУК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЗОЛОТИСТЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МИКРОСАТИН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЛИЗ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ КИЛТ/НАКИДКА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЗОЛОТОЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МИКРОФИБРА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЛАРУСЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ СПОРТИВНОЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ИЗУМРУДНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МИКРОФРЕШ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЛЬГИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ТУАЛЕТНОЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КАПУЧИНО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МОДАЛ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕНИН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРИХВАТКА КУХОННАЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КИРПИЧНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МУЛЕТОН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕРМУДЫ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ КУХОННОЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОРАЛЛОВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НЕТКАНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БОЛГАРИЯ</t>
+  </si>
+  <si>
     <t xml:space="preserve">ПРОСТЫНЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">БЕЖЕВЫЙ МЕЛАНЖ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ДЕТСКИЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">НЕ ОПРЕДЕЛЕНО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АВСТРАЛИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЖЕВЫЙ/ЗЕЛЕНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЛЮБОЙ ВОЗРАСТ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АКФИЛ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АВСТРИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сертификат</t>
-  </si>
-  <si>
-    <t xml:space="preserve">НАМАТРАСНИК</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЖЕВЫЙ/СИНИЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЗ УКАЗАНИЯ ВОЗРАСТА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АЗЕРБАЙДЖАН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Модель / артикул производителя(тип)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Модель</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КОМПЛЕКТ ПОСТЕЛЬНОГО БЕЛЬЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЛО-ЗЕЛЕНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БАЙКА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АЛАНДСКИЕ ОСТРОВА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ ГОСТЕВОЕ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЛО-КОРИЧНЕВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БАТИСТ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АЛБАНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Модель / Артикул</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КОМПЛЕКТ ПОЛОТЕНЕЦ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БИОМАТИН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АЛЖИР</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ БАННОЕ/КУПАЛЬНОЕ ПОЛОТЕНЦЕ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЛЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЯЗЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АМЕРИКАНСКИЕ ВИРГИНСКИЕ ОСТРОВА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ РУК</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЛЫЙ/БЕЖЕВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ВЕЛЮР</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АМЕРИКАНСКОЕ САМОА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ ПЛЯЖНОЕ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ВУАЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АНГИЛЬЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КОВРИК</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЛЫЙ/СИНИЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ВАФЕЛЬНОЕ ПОЛОТНО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АНГОЛА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ИЗДЕЛИЕ ДЛЯ БАНИ И САУНЫ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БИРЮЗОВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ГАБАРДИН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АНДОРРА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ДОРОЖКА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БОРДОВО-РЫЖИЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ГОБЕЛЕН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АНТАРКТИДА</t>
+    <t xml:space="preserve">КОРИЧНЕВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОРГАНЗА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БОЛИВИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОСТЫНЯ БАННАЯ/КУПАЛЬНАЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОФЕЙНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПЕРИОТЕК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БОСНИЯ И ГЕРЦЕГОВИНА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КРАСНО-КОРИЧНЕВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПЕРКАЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БОТСВАНА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">РУШНИК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КРАСНЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПИКЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БРАЗИЛИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">САЛФЕТКА ЧАЙНАЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КРЕМОВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПЛЮШ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БРИТАНСКАЯ ТЕРРИТОРИЯ В ИНДИЙСКОМ ОКЕАНЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">САЛФЕТКА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЛАВАНДОВЫЙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛИКОТТОН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БРИТАНСКИЕ ВИРГИНСКИЕ ОСТРОВА</t>
   </si>
   <si>
     <t xml:space="preserve">САЛФЕТКА ПОД ПРИБОРЫ</t>
   </si>
   <si>
-    <t xml:space="preserve">БОРДОВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ДАМАСТ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АНТИГУА И БАРБУДА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Номер Регламента/стандарта</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ТР ТС 007/2011 "О безопасности продукции, предназначенной для детей и подростков"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">САЛФЕТКА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БРОНЗОВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ДЖЕРСИ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АРГЕНТИНА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ТР ТС 017/2011 "О безопасности продукции легкой промышленности"</t>
+    <t xml:space="preserve">ЛАЙМ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛИПРОПИЛЕН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БРУНЕЙ ДАРУССАЛАМ</t>
   </si>
   <si>
     <t xml:space="preserve">СКАТЕРТЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">ВАНИЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЖАККАРД</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АРМЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ТР ТС 005/2011 "О безопасности упаковки"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ВИШНЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КУЛИРНАЯ ГЛАДЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АРУБА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Действие технических регламентов не распространяется</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ГОЛУБОЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЛЬНЯНАЯ ТКАНЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">АФГАНИСТАН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ГОРЧИЧНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МАКО-САТИН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БАГАМЫ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ГРАФИТОВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МАХРОВАЯ ТКАНЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БАНГЛАДЕШ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЖЁЛТЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МИКРОВОЛОКНО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БАРБАДОС</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЗЕЛЁНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МИКРОПОЛИЕСТР</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БАХРЕЙН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЗОЛОТИСТЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МИКРОСАТИН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЛИЗ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЗОЛОТОЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МИКРОФИБРА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЛАРУСЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ИЗУМРУДНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МИКРОФРЕШ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕЛЬГИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КАПУЧИНО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МОДАЛ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕНИН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КИРПИЧНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">МУЛЕТОН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БЕРМУДЫ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КОРАЛЛОВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">НЕТКАНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БОЛГАРИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КОРИЧНЕВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОРГАНЗА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БОЛИВИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КОФЕЙНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПЕРИОТЕК</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БОСНИЯ И ГЕРЦЕГОВИНА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КРАСНО-КОРИЧНЕВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПЕРКАЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БОТСВАНА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КРАСНЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПИКЕ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БРАЗИЛИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КРЕМОВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПЛЮШ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БРИТАНСКАЯ ТЕРРИТОРИЯ В ИНДИЙСКОМ ОКЕАНЕ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЛАВАНДОВЫЙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛИКОТТОН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БРИТАНСКИЕ ВИРГИНСКИЕ ОСТРОВА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЛАЙМ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛИПРОПИЛЕН</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БРУНЕЙ ДАРУССАЛАМ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ЛЕОПАРД</t>
   </si>
   <si>
@@ -666,6 +729,9 @@
     <t xml:space="preserve">БУРКИНА-ФАСО</t>
   </si>
   <si>
+    <t xml:space="preserve">ФАРТУК</t>
+  </si>
+  <si>
     <t xml:space="preserve">МАЛИНОВЫЙ</t>
   </si>
   <si>
@@ -675,6 +741,9 @@
     <t xml:space="preserve">БУРУНДИ</t>
   </si>
   <si>
+    <t xml:space="preserve">ХАЛАТ</t>
+  </si>
+  <si>
     <t xml:space="preserve">МЕДНЫЙ</t>
   </si>
   <si>
@@ -684,6 +753,9 @@
     <t xml:space="preserve">БУТАН</t>
   </si>
   <si>
+    <t xml:space="preserve">ЧЕХОЛ</t>
+  </si>
+  <si>
     <t xml:space="preserve">МОЛОЧНЫЙ</t>
   </si>
   <si>
@@ -691,6 +763,9 @@
   </si>
   <si>
     <t xml:space="preserve">ВАНУАТУ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЮБКА ДЛЯ СТОЛА</t>
   </si>
   <si>
     <t xml:space="preserve">МЯТНЫЙ</t>
@@ -2850,7 +2925,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2965,6 +3040,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -3088,16 +3167,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1752"/>
+  <dimension ref="A1:AMJ1831"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="47.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="27.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="34.53"/>
@@ -34035,6 +34114,243 @@
     <row r="1752" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F1752" s="17"/>
     </row>
+    <row r="1753" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1753" s="17"/>
+    </row>
+    <row r="1754" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1754" s="17"/>
+    </row>
+    <row r="1755" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1755" s="17"/>
+    </row>
+    <row r="1756" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1756" s="17"/>
+    </row>
+    <row r="1757" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1757" s="17"/>
+    </row>
+    <row r="1758" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1758" s="17"/>
+    </row>
+    <row r="1759" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1759" s="17"/>
+    </row>
+    <row r="1760" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1760" s="17"/>
+    </row>
+    <row r="1761" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1761" s="17"/>
+    </row>
+    <row r="1762" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1762" s="17"/>
+    </row>
+    <row r="1763" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1763" s="17"/>
+    </row>
+    <row r="1764" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1764" s="17"/>
+    </row>
+    <row r="1765" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1765" s="17"/>
+    </row>
+    <row r="1766" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1766" s="17"/>
+    </row>
+    <row r="1767" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1767" s="17"/>
+    </row>
+    <row r="1768" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1768" s="17"/>
+    </row>
+    <row r="1769" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1769" s="17"/>
+    </row>
+    <row r="1770" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1770" s="17"/>
+    </row>
+    <row r="1771" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1771" s="17"/>
+    </row>
+    <row r="1772" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1772" s="17"/>
+    </row>
+    <row r="1773" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1773" s="17"/>
+    </row>
+    <row r="1774" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1774" s="17"/>
+    </row>
+    <row r="1775" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1775" s="17"/>
+    </row>
+    <row r="1776" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1776" s="17"/>
+    </row>
+    <row r="1777" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1777" s="17"/>
+    </row>
+    <row r="1778" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1778" s="17"/>
+    </row>
+    <row r="1779" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1779" s="17"/>
+    </row>
+    <row r="1780" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1780" s="17"/>
+    </row>
+    <row r="1781" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1781" s="17"/>
+    </row>
+    <row r="1782" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1782" s="17"/>
+    </row>
+    <row r="1783" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1783" s="17"/>
+    </row>
+    <row r="1784" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1784" s="17"/>
+    </row>
+    <row r="1785" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1785" s="17"/>
+    </row>
+    <row r="1786" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1786" s="17"/>
+    </row>
+    <row r="1787" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1787" s="17"/>
+    </row>
+    <row r="1788" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1788" s="17"/>
+    </row>
+    <row r="1789" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1789" s="17"/>
+    </row>
+    <row r="1790" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1790" s="17"/>
+    </row>
+    <row r="1791" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1791" s="17"/>
+    </row>
+    <row r="1792" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1792" s="17"/>
+    </row>
+    <row r="1793" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1793" s="17"/>
+    </row>
+    <row r="1794" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1794" s="17"/>
+    </row>
+    <row r="1795" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1795" s="17"/>
+    </row>
+    <row r="1796" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1796" s="17"/>
+    </row>
+    <row r="1797" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1797" s="17"/>
+    </row>
+    <row r="1798" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1798" s="17"/>
+    </row>
+    <row r="1799" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1799" s="17"/>
+    </row>
+    <row r="1800" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1800" s="17"/>
+    </row>
+    <row r="1801" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1801" s="17"/>
+    </row>
+    <row r="1802" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1802" s="17"/>
+    </row>
+    <row r="1803" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1803" s="17"/>
+    </row>
+    <row r="1804" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1804" s="17"/>
+    </row>
+    <row r="1805" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1805" s="17"/>
+    </row>
+    <row r="1806" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1806" s="17"/>
+    </row>
+    <row r="1807" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1807" s="17"/>
+    </row>
+    <row r="1808" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1808" s="17"/>
+    </row>
+    <row r="1809" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1809" s="17"/>
+    </row>
+    <row r="1810" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1810" s="17"/>
+    </row>
+    <row r="1811" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1811" s="17"/>
+    </row>
+    <row r="1812" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1812" s="17"/>
+    </row>
+    <row r="1813" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1813" s="17"/>
+    </row>
+    <row r="1814" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1814" s="17"/>
+    </row>
+    <row r="1815" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1815" s="17"/>
+    </row>
+    <row r="1816" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1816" s="17"/>
+    </row>
+    <row r="1817" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1817" s="17"/>
+    </row>
+    <row r="1818" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1818" s="17"/>
+    </row>
+    <row r="1819" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1819" s="17"/>
+    </row>
+    <row r="1820" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1820" s="17"/>
+    </row>
+    <row r="1821" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1821" s="17"/>
+    </row>
+    <row r="1822" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1822" s="17"/>
+    </row>
+    <row r="1823" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1823" s="17"/>
+    </row>
+    <row r="1824" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1824" s="17"/>
+    </row>
+    <row r="1825" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1825" s="17"/>
+    </row>
+    <row r="1826" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1826" s="17"/>
+    </row>
+    <row r="1827" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1827" s="17"/>
+    </row>
+    <row r="1828" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1828" s="17"/>
+    </row>
+    <row r="1829" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1829" s="17"/>
+    </row>
+    <row r="1830" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1830" s="17"/>
+    </row>
+    <row r="1831" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1831" s="17"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:E1"/>
@@ -34042,10 +34358,6 @@
     <mergeCell ref="Q6:S6"/>
   </mergeCells>
   <dataValidations count="9">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F7:F1752" type="list">
-      <formula1>Справочники!$D$2:$D$33</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6" type="textLength">
       <formula1>1025</formula1>
       <formula2>0</formula2>
@@ -34078,6 +34390,10 @@
       <formula1>Справочники!$F$2:$F$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F7:F1831" type="list">
+      <formula1>Справочники!$D$2:$D$41</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -34096,11 +34412,11 @@
   </sheetPr>
   <dimension ref="A1:I246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="24.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="49.34"/>
@@ -34138,45 +34454,45 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="7" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>57</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I3" s="27" t="s">
         <v>64</v>
@@ -34184,925 +34500,996 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="7" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>70</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="E20" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="E21" s="7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="7" t="s">
+        <v>170</v>
+      </c>
       <c r="E22" s="7" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="7" t="s">
+        <v>174</v>
+      </c>
       <c r="E23" s="7" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="7" t="s">
+        <v>178</v>
+      </c>
       <c r="E24" s="7" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="E25" s="7" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="7" t="s">
+        <v>186</v>
+      </c>
       <c r="E26" s="7" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="H26" s="26" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="7" t="s">
+        <v>190</v>
+      </c>
       <c r="E27" s="7" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="H27" s="26" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="7" t="s">
+        <v>194</v>
+      </c>
       <c r="E28" s="7" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="H28" s="26" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="7" t="s">
+        <v>198</v>
+      </c>
       <c r="E29" s="7" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="7" t="s">
+        <v>202</v>
+      </c>
       <c r="E30" s="7" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="H30" s="26" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D31" s="7" t="s">
+        <v>206</v>
+      </c>
       <c r="E31" s="7" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="H31" s="26" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="E32" s="7" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="0"/>
+      <c r="D33" s="29" t="s">
+        <v>213</v>
+      </c>
       <c r="E33" s="7" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="H33" s="26" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="7" t="s">
+        <v>217</v>
+      </c>
       <c r="E34" s="7" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="H34" s="26" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D35" s="7" t="s">
+        <v>221</v>
+      </c>
       <c r="E35" s="7" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="H35" s="26" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D36" s="7" t="s">
+        <v>225</v>
+      </c>
       <c r="E36" s="7" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="H36" s="26" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="7" t="s">
+        <v>229</v>
+      </c>
       <c r="E37" s="7" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="H37" s="26" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="7" t="s">
+        <v>233</v>
+      </c>
       <c r="E38" s="7" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="E39" s="7" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="7" t="s">
+        <v>241</v>
+      </c>
       <c r="E40" s="7" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="7" t="s">
+        <v>245</v>
+      </c>
       <c r="E41" s="7" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>223</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="7" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="H42" s="26" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="7" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="7" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="H44" s="26" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="7" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
       <c r="H45" s="26" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="7" t="s">
-        <v>236</v>
+        <v>261</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="7" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="H47" s="26" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="7" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="H48" s="26" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="7" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="7" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="7" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="H51" s="26" t="s">
-        <v>253</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="7" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="H52" s="26" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="7" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="7" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>261</v>
+        <v>286</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>262</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="7" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>264</v>
+        <v>289</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="7" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="7" t="s">
-        <v>269</v>
+        <v>294</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>270</v>
+        <v>295</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>271</v>
+        <v>296</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="7" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="7" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="7" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="7" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="7" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="H62" s="26" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="7" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="7" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>292</v>
+        <v>317</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="7" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="H65" s="26" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="7" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>297</v>
+        <v>322</v>
       </c>
       <c r="H66" s="26" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="7" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
       <c r="H67" s="26" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="7" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="7" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="H69" s="26" t="s">
-        <v>305</v>
+        <v>330</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="7" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="H70" s="26" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="7" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="H71" s="26" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="7" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
       <c r="H72" s="26" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="7" t="s">
-        <v>312</v>
+        <v>337</v>
       </c>
       <c r="H73" s="26" t="s">
-        <v>313</v>
+        <v>338</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="7" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
       <c r="H74" s="26" t="s">
-        <v>315</v>
+        <v>340</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="7" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="H75" s="26" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="7" t="s">
-        <v>318</v>
+        <v>343</v>
       </c>
       <c r="H76" s="26" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="7" t="s">
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="H77" s="26" t="s">
-        <v>321</v>
+        <v>346</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="7" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="H78" s="26" t="s">
-        <v>323</v>
+        <v>348</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="7" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
       <c r="H79" s="26" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="7" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="H80" s="26" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="7" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="H81" s="26" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="7" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="H82" s="26" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="7" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="H83" s="26" t="s">
         <v>74</v>
@@ -35110,103 +35497,103 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="7" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="H84" s="26" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="7" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="H85" s="26" t="s">
-        <v>336</v>
+        <v>361</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="7" t="s">
-        <v>337</v>
+        <v>362</v>
       </c>
       <c r="H86" s="26" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="7" t="s">
-        <v>339</v>
+        <v>364</v>
       </c>
       <c r="H87" s="26" t="s">
-        <v>340</v>
+        <v>365</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="7" t="s">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="H88" s="26" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="7" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="H89" s="26" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="7" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
       <c r="H90" s="26" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="7" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="H91" s="26" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="7" t="s">
-        <v>349</v>
+        <v>374</v>
       </c>
       <c r="H92" s="26" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="7" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
       <c r="H93" s="26" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="7" t="s">
-        <v>353</v>
+        <v>378</v>
       </c>
       <c r="H94" s="26" t="s">
-        <v>354</v>
+        <v>379</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="7" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
       <c r="H95" s="26" t="s">
-        <v>356</v>
+        <v>381</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="7" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="H96" s="26" t="s">
         <v>63</v>
@@ -35214,774 +35601,774 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="7" t="s">
-        <v>358</v>
+        <v>383</v>
       </c>
       <c r="H97" s="26" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="7" t="s">
-        <v>360</v>
+        <v>385</v>
       </c>
       <c r="H98" s="26" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="7" t="s">
-        <v>362</v>
+        <v>387</v>
       </c>
       <c r="H99" s="26" t="s">
-        <v>363</v>
+        <v>388</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="7" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
       <c r="H100" s="26" t="s">
-        <v>365</v>
+        <v>390</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="7" t="s">
-        <v>366</v>
+        <v>391</v>
       </c>
       <c r="H101" s="26" t="s">
-        <v>367</v>
+        <v>392</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="7" t="s">
-        <v>368</v>
+        <v>393</v>
       </c>
       <c r="H102" s="26" t="s">
-        <v>369</v>
+        <v>394</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="7" t="s">
-        <v>370</v>
+        <v>395</v>
       </c>
       <c r="H103" s="26" t="s">
-        <v>371</v>
+        <v>396</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="7" t="s">
-        <v>372</v>
+        <v>397</v>
       </c>
       <c r="H104" s="26" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="7" t="s">
-        <v>374</v>
+        <v>399</v>
       </c>
       <c r="H105" s="26" t="s">
-        <v>375</v>
+        <v>400</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="7" t="s">
-        <v>376</v>
+        <v>401</v>
       </c>
       <c r="H106" s="26" t="s">
-        <v>377</v>
+        <v>402</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="7" t="s">
-        <v>378</v>
+        <v>403</v>
       </c>
       <c r="H107" s="26" t="s">
-        <v>379</v>
+        <v>404</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="7" t="s">
-        <v>380</v>
+        <v>405</v>
       </c>
       <c r="H108" s="26" t="s">
-        <v>381</v>
+        <v>406</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="7" t="s">
-        <v>382</v>
+        <v>407</v>
       </c>
       <c r="H109" s="26" t="s">
-        <v>383</v>
+        <v>408</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="7" t="s">
-        <v>384</v>
+        <v>409</v>
       </c>
       <c r="H110" s="26" t="s">
-        <v>385</v>
+        <v>410</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H111" s="26" t="s">
-        <v>386</v>
+        <v>411</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H112" s="26" t="s">
-        <v>387</v>
+        <v>412</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H113" s="26" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H114" s="26" t="s">
-        <v>389</v>
+        <v>414</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H115" s="26" t="s">
-        <v>390</v>
+        <v>415</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H116" s="26" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H117" s="26" t="s">
-        <v>392</v>
+        <v>417</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H118" s="26" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H119" s="26" t="s">
-        <v>394</v>
+        <v>419</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H120" s="26" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H121" s="26" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H122" s="26" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H123" s="26" t="s">
-        <v>398</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H124" s="26" t="s">
-        <v>399</v>
+        <v>424</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H125" s="26" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H126" s="26" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H127" s="26" t="s">
-        <v>402</v>
+        <v>427</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H128" s="26" t="s">
-        <v>403</v>
+        <v>428</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H129" s="26" t="s">
-        <v>404</v>
+        <v>429</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H130" s="26" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H131" s="26" t="s">
-        <v>406</v>
+        <v>431</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H132" s="26" t="s">
-        <v>407</v>
+        <v>432</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H133" s="26" t="s">
-        <v>408</v>
+        <v>433</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H134" s="26" t="s">
-        <v>409</v>
+        <v>434</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H135" s="26" t="s">
-        <v>410</v>
+        <v>435</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H136" s="26" t="s">
-        <v>411</v>
+        <v>436</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H137" s="26" t="s">
-        <v>412</v>
+        <v>437</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H138" s="26" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H139" s="26" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H140" s="26" t="s">
-        <v>415</v>
+        <v>440</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H141" s="26" t="s">
-        <v>416</v>
+        <v>441</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H142" s="26" t="s">
-        <v>417</v>
+        <v>442</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H143" s="26" t="s">
-        <v>418</v>
+        <v>443</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H144" s="26" t="s">
-        <v>419</v>
+        <v>444</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H145" s="26" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H146" s="26" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H147" s="26" t="s">
-        <v>422</v>
+        <v>447</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H148" s="26" t="s">
-        <v>423</v>
+        <v>448</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H149" s="26" t="s">
-        <v>424</v>
+        <v>449</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H150" s="26" t="s">
-        <v>425</v>
+        <v>450</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H151" s="26" t="s">
-        <v>426</v>
+        <v>451</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H152" s="26" t="s">
-        <v>427</v>
+        <v>452</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H153" s="26" t="s">
-        <v>428</v>
+        <v>453</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H154" s="26" t="s">
-        <v>429</v>
+        <v>454</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H155" s="26" t="s">
-        <v>430</v>
+        <v>455</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H156" s="26" t="s">
-        <v>431</v>
+        <v>456</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H157" s="26" t="s">
-        <v>432</v>
+        <v>457</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H158" s="26" t="s">
-        <v>433</v>
+        <v>458</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H159" s="26" t="s">
-        <v>434</v>
+        <v>459</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H160" s="26" t="s">
-        <v>435</v>
+        <v>460</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H161" s="26" t="s">
-        <v>436</v>
+        <v>461</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H162" s="26" t="s">
-        <v>437</v>
+        <v>462</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H163" s="26" t="s">
-        <v>438</v>
+        <v>463</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H164" s="26" t="s">
-        <v>439</v>
+        <v>464</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H165" s="26" t="s">
-        <v>440</v>
+        <v>465</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H166" s="26" t="s">
-        <v>441</v>
+        <v>466</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H167" s="26" t="s">
-        <v>442</v>
+        <v>467</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H168" s="26" t="s">
-        <v>443</v>
+        <v>468</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H169" s="26" t="s">
-        <v>444</v>
+        <v>469</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H170" s="26" t="s">
-        <v>445</v>
+        <v>470</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H171" s="26" t="s">
-        <v>446</v>
+        <v>471</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H172" s="26" t="s">
-        <v>447</v>
+        <v>472</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H173" s="26" t="s">
-        <v>448</v>
+        <v>473</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H174" s="26" t="s">
-        <v>449</v>
+        <v>474</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H175" s="26" t="s">
-        <v>450</v>
+        <v>475</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H176" s="26" t="s">
-        <v>451</v>
+        <v>476</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H177" s="26" t="s">
-        <v>452</v>
+        <v>477</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H178" s="26" t="s">
-        <v>453</v>
+        <v>478</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H179" s="26" t="s">
-        <v>454</v>
+        <v>479</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H180" s="26" t="s">
-        <v>455</v>
+        <v>480</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H181" s="26" t="s">
-        <v>456</v>
+        <v>481</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H182" s="26" t="s">
-        <v>457</v>
+        <v>482</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H183" s="26" t="s">
-        <v>458</v>
+        <v>483</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H184" s="26" t="s">
-        <v>459</v>
+        <v>484</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H185" s="26" t="s">
-        <v>460</v>
+        <v>485</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H186" s="26" t="s">
-        <v>461</v>
+        <v>486</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H187" s="26" t="s">
-        <v>462</v>
+        <v>487</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H188" s="26" t="s">
-        <v>463</v>
+        <v>488</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H189" s="26" t="s">
-        <v>464</v>
+        <v>489</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H190" s="26" t="s">
-        <v>465</v>
+        <v>490</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H191" s="26" t="s">
-        <v>466</v>
+        <v>491</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H192" s="26" t="s">
-        <v>467</v>
+        <v>492</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H193" s="26" t="s">
-        <v>468</v>
+        <v>493</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H194" s="26" t="s">
-        <v>469</v>
+        <v>494</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H195" s="26" t="s">
-        <v>470</v>
+        <v>495</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H196" s="26" t="s">
-        <v>471</v>
+        <v>496</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H197" s="26" t="s">
-        <v>472</v>
+        <v>497</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H198" s="26" t="s">
-        <v>473</v>
+        <v>498</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H199" s="26" t="s">
-        <v>474</v>
+        <v>499</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H200" s="26" t="s">
-        <v>475</v>
+        <v>500</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H201" s="26" t="s">
-        <v>476</v>
+        <v>501</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H202" s="26" t="s">
-        <v>477</v>
+        <v>502</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H203" s="26" t="s">
-        <v>478</v>
+        <v>503</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H204" s="26" t="s">
-        <v>479</v>
+        <v>504</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H205" s="26" t="s">
-        <v>480</v>
+        <v>505</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H206" s="26" t="s">
-        <v>481</v>
+        <v>506</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H207" s="26" t="s">
-        <v>482</v>
+        <v>507</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H208" s="26" t="s">
-        <v>483</v>
+        <v>508</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H209" s="26" t="s">
-        <v>484</v>
+        <v>509</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H210" s="26" t="s">
-        <v>485</v>
+        <v>510</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H211" s="26" t="s">
-        <v>486</v>
+        <v>511</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H212" s="26" t="s">
-        <v>487</v>
+        <v>512</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H213" s="26" t="s">
-        <v>488</v>
+        <v>513</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H214" s="26" t="s">
-        <v>489</v>
+        <v>514</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H215" s="26" t="s">
-        <v>490</v>
+        <v>515</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H216" s="26" t="s">
-        <v>491</v>
+        <v>516</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H217" s="26" t="s">
-        <v>492</v>
+        <v>517</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H218" s="26" t="s">
-        <v>493</v>
+        <v>518</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H219" s="26" t="s">
-        <v>494</v>
+        <v>519</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H220" s="26" t="s">
-        <v>495</v>
+        <v>520</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H221" s="26" t="s">
-        <v>496</v>
+        <v>521</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H222" s="26" t="s">
-        <v>497</v>
+        <v>522</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H223" s="26" t="s">
-        <v>498</v>
+        <v>523</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H224" s="26" t="s">
-        <v>499</v>
+        <v>524</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H225" s="26" t="s">
-        <v>500</v>
+        <v>525</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H226" s="26" t="s">
-        <v>501</v>
+        <v>526</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H227" s="26" t="s">
-        <v>502</v>
+        <v>527</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H228" s="26" t="s">
-        <v>503</v>
+        <v>528</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H229" s="26" t="s">
-        <v>504</v>
+        <v>529</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H230" s="26" t="s">
-        <v>505</v>
+        <v>530</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H231" s="26" t="s">
-        <v>506</v>
+        <v>531</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H232" s="26" t="s">
-        <v>507</v>
+        <v>532</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H233" s="26" t="s">
-        <v>508</v>
+        <v>533</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H234" s="26" t="s">
-        <v>509</v>
+        <v>534</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H235" s="26" t="s">
-        <v>510</v>
+        <v>535</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H236" s="26" t="s">
-        <v>511</v>
+        <v>536</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H237" s="26" t="s">
-        <v>512</v>
+        <v>537</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H238" s="26" t="s">
-        <v>513</v>
+        <v>538</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H239" s="26" t="s">
-        <v>514</v>
+        <v>539</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H240" s="26" t="s">
-        <v>515</v>
+        <v>540</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H241" s="26" t="s">
-        <v>516</v>
+        <v>541</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H242" s="26" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36024,26 +36411,26 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="53.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>518</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>519</v>
+      <c r="A1" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="n">
+      <c r="A2" s="32" t="n">
         <v>4203</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>520</v>
+      <c r="B2" s="33" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36051,7 +36438,7 @@
         <v>4203100001</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>521</v>
+        <v>546</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36059,31 +36446,31 @@
         <v>4203100009</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>522</v>
+        <v>547</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="n">
+      <c r="A5" s="32" t="n">
         <v>6106</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>523</v>
+      <c r="B5" s="33" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>6106100000</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>524</v>
+      <c r="B6" s="34" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>6106200000</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>525</v>
+      <c r="B7" s="34" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36091,7 +36478,7 @@
         <v>6106901000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>526</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36099,7 +36486,7 @@
         <v>6106903000</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>527</v>
+        <v>552</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36107,7 +36494,7 @@
         <v>6106905000</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>528</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36115,15 +36502,15 @@
         <v>6106909000</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>529</v>
+        <v>554</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31" t="n">
+      <c r="A12" s="32" t="n">
         <v>6201</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>530</v>
+      <c r="B12" s="33" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36131,7 +36518,7 @@
         <v>6201200000</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>531</v>
+        <v>556</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36139,7 +36526,7 @@
         <v>6201300000</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>532</v>
+        <v>557</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36147,7 +36534,7 @@
         <v>6201400000</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>533</v>
+        <v>558</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36155,15 +36542,15 @@
         <v>6201900000</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>534</v>
+        <v>559</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31" t="n">
+      <c r="A17" s="32" t="n">
         <v>6202</v>
       </c>
-      <c r="B17" s="32" t="s">
-        <v>535</v>
+      <c r="B17" s="33" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36171,7 +36558,7 @@
         <v>6202200000</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>536</v>
+        <v>561</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36179,7 +36566,7 @@
         <v>6202300000</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>537</v>
+        <v>562</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36187,7 +36574,7 @@
         <v>6202400001</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>538</v>
+        <v>563</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36195,7 +36582,7 @@
         <v>6202400009</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>539</v>
+        <v>564</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36203,7 +36590,7 @@
         <v>6202900001</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>540</v>
+        <v>565</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36211,15 +36598,15 @@
         <v>6202900009</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>541</v>
+        <v>566</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31" t="n">
+      <c r="A24" s="32" t="n">
         <v>6302</v>
       </c>
-      <c r="B24" s="32" t="s">
-        <v>542</v>
+      <c r="B24" s="33" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36227,7 +36614,7 @@
         <v>6302100001</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>543</v>
+        <v>568</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36235,7 +36622,7 @@
         <v>6302100009</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>544</v>
+        <v>569</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36243,7 +36630,7 @@
         <v>6302210000</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>545</v>
+        <v>570</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36251,7 +36638,7 @@
         <v>6302221000</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>546</v>
+        <v>571</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36259,7 +36646,7 @@
         <v>6302229000</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36267,7 +36654,7 @@
         <v>6302310001</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>548</v>
+        <v>573</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36275,7 +36662,7 @@
         <v>6302310009</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>549</v>
+        <v>574</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36283,7 +36670,7 @@
         <v>6302321000</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>550</v>
+        <v>575</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36291,7 +36678,7 @@
         <v>6302329000</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>551</v>
+        <v>576</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36299,7 +36686,7 @@
         <v>6302392001</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>552</v>
+        <v>577</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36307,7 +36694,7 @@
         <v>6302392009</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>553</v>
+        <v>578</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36315,7 +36702,7 @@
         <v>6302399000</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>554</v>
+        <v>579</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36323,7 +36710,7 @@
         <v>6302400000</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>555</v>
+        <v>580</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36331,7 +36718,7 @@
         <v>6302510001</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>556</v>
+        <v>581</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36339,7 +36726,7 @@
         <v>6302510009</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>557</v>
+        <v>582</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36347,7 +36734,7 @@
         <v>6302531000</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>558</v>
+        <v>583</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36355,7 +36742,7 @@
         <v>6302539000</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>559</v>
+        <v>584</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36363,7 +36750,7 @@
         <v>6302591000</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>560</v>
+        <v>585</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36371,7 +36758,7 @@
         <v>6302599000</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>561</v>
+        <v>586</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36379,7 +36766,7 @@
         <v>6302600000</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>562</v>
+        <v>587</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36387,7 +36774,7 @@
         <v>6302910000</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>563</v>
+        <v>588</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36395,7 +36782,7 @@
         <v>6302931000</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>564</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36403,7 +36790,7 @@
         <v>6302939000</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>565</v>
+        <v>590</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36411,7 +36798,7 @@
         <v>6302991000</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>566</v>
+        <v>591</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36419,15 +36806,15 @@
         <v>6302999000</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>567</v>
+        <v>592</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="31" t="n">
+      <c r="A50" s="32" t="n">
         <v>4303</v>
       </c>
-      <c r="B50" s="32" t="s">
-        <v>568</v>
+      <c r="B50" s="33" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36435,7 +36822,7 @@
         <v>4303109010</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>569</v>
+        <v>594</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36443,7 +36830,7 @@
         <v>4303109020</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>570</v>
+        <v>595</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36451,7 +36838,7 @@
         <v>4303109030</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>571</v>
+        <v>596</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36459,7 +36846,7 @@
         <v>4303109040</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>572</v>
+        <v>597</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36467,7 +36854,7 @@
         <v>4303109050</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>573</v>
+        <v>598</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36475,7 +36862,7 @@
         <v>4303109060</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>574</v>
+        <v>599</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36483,15 +36870,15 @@
         <v>4303109080</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>575</v>
+        <v>600</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="31" t="n">
+      <c r="A58" s="32" t="n">
         <v>3303</v>
       </c>
-      <c r="B58" s="34" t="s">
-        <v>576</v>
+      <c r="B58" s="35" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36499,7 +36886,7 @@
         <v>3303001000</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>577</v>
+        <v>602</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36507,15 +36894,15 @@
         <v>3303009000</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>578</v>
+        <v>603</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="31" t="n">
+      <c r="A61" s="32" t="n">
         <v>4011</v>
       </c>
-      <c r="B61" s="32" t="s">
-        <v>579</v>
+      <c r="B61" s="33" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36523,7 +36910,7 @@
         <v>4011100003</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>580</v>
+        <v>605</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36531,7 +36918,7 @@
         <v>4011100009</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>581</v>
+        <v>606</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36539,7 +36926,7 @@
         <v>4011201000</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>582</v>
+        <v>607</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36547,7 +36934,7 @@
         <v>4011209000</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>583</v>
+        <v>608</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36555,7 +36942,7 @@
         <v>4011400000</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>584</v>
+        <v>609</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36563,7 +36950,7 @@
         <v>4011700000</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>585</v>
+        <v>610</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36571,7 +36958,7 @@
         <v>4011800000</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>586</v>
+        <v>611</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36579,15 +36966,15 @@
         <v>4011900000</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>587</v>
+        <v>612</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="31" t="n">
+      <c r="A70" s="32" t="n">
         <v>6401</v>
       </c>
-      <c r="B70" s="32" t="s">
-        <v>588</v>
+      <c r="B70" s="33" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36595,7 +36982,7 @@
         <v>6401100000</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>589</v>
+        <v>614</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36603,7 +36990,7 @@
         <v>6401921000</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>590</v>
+        <v>615</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36611,7 +36998,7 @@
         <v>6401929000</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>591</v>
+        <v>616</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36619,15 +37006,15 @@
         <v>6401990000</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>592</v>
+        <v>617</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="31" t="n">
+      <c r="A75" s="32" t="n">
         <v>6402</v>
       </c>
-      <c r="B75" s="32" t="s">
-        <v>593</v>
+      <c r="B75" s="33" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36635,7 +37022,7 @@
         <v>6402121000</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>594</v>
+        <v>619</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36643,7 +37030,7 @@
         <v>6402129000</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>595</v>
+        <v>620</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36651,7 +37038,7 @@
         <v>6402190000</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>596</v>
+        <v>621</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36659,7 +37046,7 @@
         <v>6402200000</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>597</v>
+        <v>622</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36667,7 +37054,7 @@
         <v>6402911000</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>598</v>
+        <v>623</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36675,7 +37062,7 @@
         <v>6402919000</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>599</v>
+        <v>624</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36683,7 +37070,7 @@
         <v>6402990500</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>600</v>
+        <v>625</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36691,7 +37078,7 @@
         <v>6402991000</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>601</v>
+        <v>626</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36699,7 +37086,7 @@
         <v>6402993100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>602</v>
+        <v>627</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36707,7 +37094,7 @@
         <v>6402993900</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>603</v>
+        <v>628</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36715,7 +37102,7 @@
         <v>6402995000</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>604</v>
+        <v>629</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36723,7 +37110,7 @@
         <v>6402999100</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>605</v>
+        <v>630</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36731,7 +37118,7 @@
         <v>6402999300</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>606</v>
+        <v>631</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36739,7 +37126,7 @@
         <v>6402999600</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>607</v>
+        <v>632</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36747,15 +37134,15 @@
         <v>6402999800</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>607</v>
+        <v>632</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="31" t="n">
+      <c r="A91" s="32" t="n">
         <v>6403</v>
       </c>
-      <c r="B91" s="32" t="s">
-        <v>608</v>
+      <c r="B91" s="33" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36763,7 +37150,7 @@
         <v>6403120000</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>609</v>
+        <v>634</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36771,7 +37158,7 @@
         <v>6403190000</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>610</v>
+        <v>635</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36779,7 +37166,7 @@
         <v>6403200000</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36787,7 +37174,7 @@
         <v>6403400000</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>612</v>
+        <v>637</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36795,7 +37182,7 @@
         <v>6403510500</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>613</v>
+        <v>638</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36803,7 +37190,7 @@
         <v>6403511100</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>614</v>
+        <v>639</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36811,7 +37198,7 @@
         <v>6403511500</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>615</v>
+        <v>640</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36819,7 +37206,7 @@
         <v>6403511900</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>616</v>
+        <v>641</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36827,7 +37214,7 @@
         <v>6403519100</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>617</v>
+        <v>642</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36835,7 +37222,7 @@
         <v>6403519500</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>618</v>
+        <v>643</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36843,7 +37230,7 @@
         <v>6403519900</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>619</v>
+        <v>644</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36851,7 +37238,7 @@
         <v>6403590500</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>620</v>
+        <v>645</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36859,7 +37246,7 @@
         <v>6403591100</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>621</v>
+        <v>646</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36867,7 +37254,7 @@
         <v>6403593100</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>622</v>
+        <v>647</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36875,7 +37262,7 @@
         <v>6403593500</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>623</v>
+        <v>648</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36883,7 +37270,7 @@
         <v>6403593900</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>624</v>
+        <v>649</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36891,7 +37278,7 @@
         <v>6403595000</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>625</v>
+        <v>650</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36899,7 +37286,7 @@
         <v>6403599100</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>626</v>
+        <v>651</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36907,7 +37294,7 @@
         <v>6403599500</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>627</v>
+        <v>652</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36915,23 +37302,23 @@
         <v>6403599900</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>628</v>
+        <v>653</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="35" t="n">
+      <c r="A112" s="36" t="n">
         <v>6403910500</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>629</v>
+        <v>654</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="35" t="n">
+      <c r="A113" s="36" t="n">
         <v>6403911100</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>630</v>
+        <v>655</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36939,7 +37326,7 @@
         <v>6403911300</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>631</v>
+        <v>656</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36947,7 +37334,7 @@
         <v>6403911600</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>632</v>
+        <v>657</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36955,7 +37342,7 @@
         <v>6403911800</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>633</v>
+        <v>658</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36963,7 +37350,7 @@
         <v>6403919100</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>634</v>
+        <v>659</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36971,7 +37358,7 @@
         <v>6403919300</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>635</v>
+        <v>660</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36979,7 +37366,7 @@
         <v>6403919600</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>636</v>
+        <v>661</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36987,7 +37374,7 @@
         <v>6403919800</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>637</v>
+        <v>662</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36995,7 +37382,7 @@
         <v>6403990500</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>638</v>
+        <v>663</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37003,7 +37390,7 @@
         <v>6403991100</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>639</v>
+        <v>664</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37011,7 +37398,7 @@
         <v>6403993100</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>640</v>
+        <v>665</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37019,7 +37406,7 @@
         <v>6403993300</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>641</v>
+        <v>666</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37027,7 +37414,7 @@
         <v>6403993600</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>642</v>
+        <v>667</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37035,7 +37422,7 @@
         <v>6403993800</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>643</v>
+        <v>668</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37043,7 +37430,7 @@
         <v>6403995000</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>644</v>
+        <v>669</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37051,7 +37438,7 @@
         <v>6403999100</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>645</v>
+        <v>670</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37059,7 +37446,7 @@
         <v>6403999300</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>646</v>
+        <v>671</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37067,7 +37454,7 @@
         <v>6403999600</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>647</v>
+        <v>672</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37075,15 +37462,15 @@
         <v>6403999800</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>648</v>
+        <v>673</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="31" t="n">
+      <c r="A132" s="32" t="n">
         <v>6404</v>
       </c>
-      <c r="B132" s="32" t="s">
-        <v>649</v>
+      <c r="B132" s="33" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37091,7 +37478,7 @@
         <v>6404110000</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>650</v>
+        <v>675</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37099,7 +37486,7 @@
         <v>6404191000</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>651</v>
+        <v>676</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37107,7 +37494,7 @@
         <v>6404199000</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>652</v>
+        <v>677</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37115,7 +37502,7 @@
         <v>6404191000</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>653</v>
+        <v>678</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37123,15 +37510,15 @@
         <v>6404209000</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>654</v>
+        <v>679</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="31" t="n">
+      <c r="A138" s="32" t="n">
         <v>6405</v>
       </c>
-      <c r="B138" s="32" t="s">
-        <v>655</v>
+      <c r="B138" s="33" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37139,7 +37526,7 @@
         <v>6405100001</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>656</v>
+        <v>681</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37147,7 +37534,7 @@
         <v>6405100009</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>657</v>
+        <v>682</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37155,7 +37542,7 @@
         <v>6405201000</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>658</v>
+        <v>683</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37163,7 +37550,7 @@
         <v>6405209100</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>659</v>
+        <v>684</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37171,7 +37558,7 @@
         <v>6405209900</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>660</v>
+        <v>685</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37179,7 +37566,7 @@
         <v>6405901000</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>661</v>
+        <v>686</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37187,7 +37574,7 @@
         <v>6405909000</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>662</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>